<commit_message>
readme + images +xlsx
</commit_message>
<xml_diff>
--- a/raci.xlsx
+++ b/raci.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivien Mouret\Documents\Ynov\PROJET_SIX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivien Mouret\Documents\Ynov\cahier_de_charge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{426C1FDA-8A95-4909-B5C9-16313699AFDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725AF30B-E25D-404D-947F-F869F5DA48E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BA27D3E2-45E9-4BE4-9A70-ACABEE04B1BD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>Qui ?</t>
   </si>
@@ -48,15 +48,6 @@
     <t>MOE</t>
   </si>
   <si>
-    <t>AMOE</t>
-  </si>
-  <si>
-    <t>MOA</t>
-  </si>
-  <si>
-    <t>AMOA</t>
-  </si>
-  <si>
     <t>besoin</t>
   </si>
   <si>
@@ -79,6 +70,18 @@
   </si>
   <si>
     <t>R/A</t>
+  </si>
+  <si>
+    <t>MOE (nous)</t>
+  </si>
+  <si>
+    <t>AMOE (nos employés)</t>
+  </si>
+  <si>
+    <t>AMOA (quartpi)</t>
+  </si>
+  <si>
+    <t>MOA (ake michi)</t>
   </si>
 </sst>
 </file>
@@ -433,12 +436,15 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -451,47 +457,47 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -499,33 +505,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
@@ -533,16 +539,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -553,13 +559,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -567,16 +573,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>

</xml_diff>